<commit_message>
First take on tabularizing a data hash. Produces mostly correct output but no headers.
</commit_message>
<xml_diff>
--- a/test/content/placeholders.xlsx
+++ b/test/content/placeholders.xlsx
@@ -485,10 +485,10 @@
   <dimension ref="A5:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.31"/>
   </cols>

</xml_diff>

<commit_message>
remove merged cells in fixture workbook
</commit_message>
<xml_diff>
--- a/test/content/placeholders.xlsx
+++ b/test/content/placeholders.xlsx
@@ -485,10 +485,10 @@
   <dimension ref="A5:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.31"/>
   </cols>
@@ -822,7 +822,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E5:F5"/>
@@ -832,7 +832,6 @@
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:K18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>